<commit_message>
Buscando voos e organizando em base de dados.
</commit_message>
<xml_diff>
--- a/ids_base_pilotos.xlsx
+++ b/ids_base_pilotos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SincFolder\Pessoais\ProjetosdeSoftware\06 - Apurador Python Liga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D11770-90AD-4228-BACD-56B718D063BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{35845378-9F48-496B-B8EA-7F755B78CDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2C26F34D-C4B1-4C51-B44C-6A844DB70497}"/>
   </bookViews>
@@ -25,71 +25,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="103">
   <si>
     <t>Nome</t>
   </si>
   <si>
-    <t>Jeferson Felicio</t>
-  </si>
-  <si>
     <t>Bernardo Margotto</t>
   </si>
   <si>
-    <t>Rony Carminati</t>
-  </si>
-  <si>
     <t>Adelso Boecker</t>
   </si>
   <si>
     <t>Marjo Lemos</t>
   </si>
   <si>
-    <t>Helio Lima</t>
-  </si>
-  <si>
-    <t>Marlos Janut</t>
-  </si>
-  <si>
-    <t>Lucas Porto</t>
-  </si>
-  <si>
-    <t>Vinicius Bianchi</t>
-  </si>
-  <si>
-    <t>Filipe Perini</t>
-  </si>
-  <si>
     <t>Mateus Haase</t>
   </si>
   <si>
-    <t>Rubens Schunk</t>
-  </si>
-  <si>
     <t>Vantuil Mataveli</t>
   </si>
   <si>
-    <t>Daniel Trevizani</t>
-  </si>
-  <si>
-    <t>Claudinei Inocente</t>
-  </si>
-  <si>
-    <t>Leomar Guilherme</t>
-  </si>
-  <si>
     <t>Leandro Schmidt</t>
   </si>
   <si>
-    <t>Ney Oliveira</t>
-  </si>
-  <si>
     <t>ID_XCBrasil</t>
   </si>
   <si>
-    <t>Andre Stavrakas</t>
-  </si>
-  <si>
     <t>0_2230</t>
   </si>
   <si>
@@ -105,15 +66,9 @@
     <t>0_6281</t>
   </si>
   <si>
-    <t>SEM</t>
-  </si>
-  <si>
     <t>0_7421</t>
   </si>
   <si>
-    <t>0_8710</t>
-  </si>
-  <si>
     <t>0_7757</t>
   </si>
   <si>
@@ -213,13 +168,172 @@
     <t>Sol - Sycross</t>
   </si>
   <si>
-    <t>Sol - Atmus 2</t>
-  </si>
-  <si>
     <t>Categoria</t>
   </si>
   <si>
-    <t>Vinicius Sassapo</t>
+    <t xml:space="preserve">Aloísio de Almeida </t>
+  </si>
+  <si>
+    <t>André Stavrakas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Claudinei Inocente </t>
+  </si>
+  <si>
+    <t>Daniel Bernardino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniel Trevezani </t>
+  </si>
+  <si>
+    <t>Eucleber Ferreira</t>
+  </si>
+  <si>
+    <t>Eumácio Versiani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filipe Perini </t>
+  </si>
+  <si>
+    <t>Hélio Lima</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Higor Penitenti </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jefferson Felicio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">João Lazarone </t>
+  </si>
+  <si>
+    <t>José Gerônimo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leomar Guilherme </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lucas Porto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manoel Junior </t>
+  </si>
+  <si>
+    <t>Marlos Janutt</t>
+  </si>
+  <si>
+    <t>Michel Pinheiro</t>
+  </si>
+  <si>
+    <t>Ney de Oliveira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rony Carminati </t>
+  </si>
+  <si>
+    <t>Rubens Schunck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruy Coelho </t>
+  </si>
+  <si>
+    <t>Sebah Freitas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silas Moreira </t>
+  </si>
+  <si>
+    <t>Thiago Werner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valentin Tesch </t>
+  </si>
+  <si>
+    <t>Vinícius Barbarioli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vinicius Bianchi </t>
+  </si>
+  <si>
+    <t>Walace de Oliveira</t>
+  </si>
+  <si>
+    <t>0_9056</t>
+  </si>
+  <si>
+    <t>0_4199</t>
+  </si>
+  <si>
+    <t>0_4579</t>
+  </si>
+  <si>
+    <t>0_9196</t>
+  </si>
+  <si>
+    <t>0_7241</t>
+  </si>
+  <si>
+    <t>0_4942</t>
+  </si>
+  <si>
+    <t>0_5311</t>
+  </si>
+  <si>
+    <t>0_9199</t>
+  </si>
+  <si>
+    <t>0_4948</t>
+  </si>
+  <si>
+    <t>0_2704</t>
+  </si>
+  <si>
+    <t>0_4844</t>
+  </si>
+  <si>
+    <t>0_3288</t>
+  </si>
+  <si>
+    <t>0_7299</t>
+  </si>
+  <si>
+    <t>0_3331</t>
+  </si>
+  <si>
+    <t>0_10484</t>
+  </si>
+  <si>
+    <t>0_4188</t>
+  </si>
+  <si>
+    <t>0_5877</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - </t>
+  </si>
+  <si>
+    <t>OZONE - Enzo 3</t>
+  </si>
+  <si>
+    <t>Ozone - Enzo 3</t>
+  </si>
+  <si>
+    <t>Flow - Spectra 2</t>
+  </si>
+  <si>
+    <t>Niviuk - Evox</t>
+  </si>
+  <si>
+    <t>Gin - Leopard</t>
+  </si>
+  <si>
+    <t>Sport</t>
+  </si>
+  <si>
+    <t>Sport Lite</t>
+  </si>
+  <si>
+    <t>Open</t>
   </si>
 </sst>
 </file>
@@ -572,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E4F33C-66C3-4367-9E3B-0FC7E7A95478}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,38 +706,41 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1">
         <v>44927</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>93</v>
       </c>
       <c r="C3" s="1">
         <v>44927</v>
@@ -631,257 +748,569 @@
       <c r="D3" t="s">
         <v>46</v>
       </c>
+      <c r="E3" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1">
         <v>44927</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1">
         <v>44927</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1">
         <v>44927</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="C7" s="1">
         <v>44927</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1">
         <v>44927</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="C9" s="1">
         <v>44927</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="C10" s="1">
         <v>44927</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1">
         <v>44927</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1">
         <v>44927</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C13" s="1">
         <v>44927</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="C14" s="1">
         <v>44927</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>29</v>
+      </c>
+      <c r="E14" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
       <c r="C15" s="1">
         <v>44927</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>94</v>
+      </c>
+      <c r="E15" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D20" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="1">
-        <v>44927</v>
-      </c>
-      <c r="D16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="1">
-        <v>44927</v>
-      </c>
-      <c r="D17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="C23" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D27" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="1">
-        <v>44927</v>
-      </c>
-      <c r="D18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="E27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D28" t="s">
+        <v>98</v>
+      </c>
+      <c r="E28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D29" t="s">
+        <v>97</v>
+      </c>
+      <c r="E29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D30" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D31" t="s">
+        <v>97</v>
+      </c>
+      <c r="E31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D33" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="1">
-        <v>44927</v>
-      </c>
-      <c r="D19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="E33" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D34" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="1">
-        <v>44927</v>
-      </c>
-      <c r="D20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="1">
-        <v>44927</v>
-      </c>
-      <c r="D21" t="s">
-        <v>53</v>
+      <c r="E34" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D35" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D36" t="s">
+        <v>99</v>
+      </c>
+      <c r="E36" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>